<commit_message>
all working: up to date
</commit_message>
<xml_diff>
--- a/tradept/Excel/Localization/Main/english/J集市信息表_Bazzar_hotfix.xlsx
+++ b/tradept/Excel/Localization/Main/english/J集市信息表_Bazzar_hotfix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xargs01\Downloads\trasl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\tradept\Excel\Localization\Main\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311834E8-5EC5-4877-99F1-1BEA6FE94655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972E3A83-A8FB-410F-B81A-89E5F46F0ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="750" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -96,43 +96,43 @@
     <t>通用赫炎雇佣兵</t>
   </si>
   <si>
-    <t>Redstone Keep: Bazar de artesanos</t>
-  </si>
-  <si>
-    <t>Frost Valley: Bazar de la Rosa Blanca</t>
-  </si>
-  <si>
-    <t>Diresprings: Bazar del Desierto</t>
-  </si>
-  <si>
     <t>Fleur: Bazar de Flores</t>
   </si>
   <si>
-    <t>Punto de interés</t>
-  </si>
-  <si>
-    <t>Comerciante de habilidades</t>
-  </si>
-  <si>
-    <t>Comerciante Viajero 1</t>
-  </si>
-  <si>
-    <t>Comerciante Viajero 2</t>
-  </si>
-  <si>
-    <t>Comerciante Viajero Senior 1</t>
-  </si>
-  <si>
-    <t>Comerciante de Bestias Común</t>
-  </si>
-  <si>
-    <t>Mercenario de Rosa Blanca Común</t>
-  </si>
-  <si>
-    <t>Mercenario de Mastigure Común</t>
-  </si>
-  <si>
-    <t>Mercenario Ember Común</t>
+    <t>Redstone Keep: Bazar dos Artesãos</t>
+  </si>
+  <si>
+    <t>Vale Frost: Bazar da Rosa Branca</t>
+  </si>
+  <si>
+    <t>Diresprings: Bazar do Deserto</t>
+  </si>
+  <si>
+    <t>Ponto de interesse</t>
+  </si>
+  <si>
+    <t>Comerciante de Habilidades</t>
+  </si>
+  <si>
+    <t>Comerciante Viajante 1</t>
+  </si>
+  <si>
+    <t>Comerciante Viajante 2</t>
+  </si>
+  <si>
+    <t>Comerciante Viajante Sênior 1</t>
+  </si>
+  <si>
+    <t>Comerciante de Bestas Comuns</t>
+  </si>
+  <si>
+    <t>Mercenário Rosa Branca Comum</t>
+  </si>
+  <si>
+    <t>Mercenário Mastigure Comum</t>
+  </si>
+  <si>
+    <t>Mercenário Brasa Comum</t>
   </si>
 </sst>
 </file>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,10 +510,13 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -534,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -545,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -556,7 +559,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -567,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>